<commit_message>
final changes for testing
</commit_message>
<xml_diff>
--- a/data/initial_state_2.xlsx
+++ b/data/initial_state_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliemacvic/Desktop/Initial States/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeboersma/School/AI Project/ai-project-post-break/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2424A-484D-6E47-9CB5-A4D858EBC4DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B07F75-BF40-AD4A-AF2F-DC6230EE59E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="460" windowWidth="23620" windowHeight="15000" xr2:uid="{ED844C13-9B21-4E40-B03F-93EF884CFD31}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,12 +473,12 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -620,7 +620,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -699,7 +699,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -770,7 +770,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -841,7 +841,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -904,8 +904,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:23" s="1" customFormat="1"/>
+    <row r="8" spans="1:23" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -919,7 +919,7 @@
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>